<commit_message>
fix finding facility center, breakdown file
</commit_message>
<xml_diff>
--- a/fixtures/output/01043110000366247_incidence.xlsx
+++ b/fixtures/output/01043110000366247_incidence.xlsx
@@ -421,10 +421,10 @@
         <v>7</v>
       </c>
       <c r="D2" t="n">
-        <v>1.76378553802e-06</v>
+        <v>1.90094648465e-06</v>
       </c>
       <c r="E2" t="n">
-        <v>1.8e-06</v>
+        <v>1.9e-06</v>
       </c>
     </row>
     <row r="3" spans="1:5">
@@ -438,10 +438,10 @@
         <v>7</v>
       </c>
       <c r="D3" t="n">
-        <v>1.76378553802e-06</v>
+        <v>1.90094648465e-06</v>
       </c>
       <c r="E3" t="n">
-        <v>1.8e-06</v>
+        <v>1.9e-06</v>
       </c>
     </row>
     <row r="4" spans="1:5">
@@ -489,10 +489,10 @@
         <v>7</v>
       </c>
       <c r="D6" t="n">
-        <v>1.76378553802e-06</v>
+        <v>1.90094648465e-06</v>
       </c>
       <c r="E6" t="n">
-        <v>1.8e-06</v>
+        <v>1.9e-06</v>
       </c>
     </row>
     <row r="7" spans="1:5">
@@ -540,10 +540,10 @@
         <v>7</v>
       </c>
       <c r="D9" t="n">
-        <v>1.76378553802e-06</v>
+        <v>1.90094648465e-06</v>
       </c>
       <c r="E9" t="n">
-        <v>1.8e-06</v>
+        <v>1.9e-06</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updated Incidence to remove single pollutant lines with inc = 0, updated test fixture as well
</commit_message>
<xml_diff>
--- a/fixtures/output/01043110000366247_incidence.xlsx
+++ b/fixtures/output/01043110000366247_incidence.xlsx
@@ -385,7 +385,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E9"/>
+  <dimension ref="A1:E7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -446,27 +446,27 @@
     </row>
     <row r="4" spans="1:5">
       <c r="A4" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="B4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C4" t="s">
         <v>7</v>
       </c>
       <c r="D4" t="n">
-        <v>0</v>
+        <v>1.90094648465e-06</v>
       </c>
       <c r="E4" t="n">
-        <v>0</v>
+        <v>1.9e-06</v>
       </c>
     </row>
     <row r="5" spans="1:5">
       <c r="A5" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="B5" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C5" t="s">
         <v>7</v>
@@ -483,66 +483,32 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="C6" t="s">
         <v>7</v>
       </c>
       <c r="D6" t="n">
-        <v>1.90094648465e-06</v>
+        <v>0</v>
       </c>
       <c r="E6" t="n">
-        <v>1.9e-06</v>
+        <v>0</v>
       </c>
     </row>
     <row r="7" spans="1:5">
       <c r="A7" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="B7" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="C7" t="s">
         <v>7</v>
       </c>
       <c r="D7" t="n">
-        <v>0</v>
+        <v>1.90094648465e-06</v>
       </c>
       <c r="E7" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5">
-      <c r="A8" t="s">
-        <v>5</v>
-      </c>
-      <c r="B8" t="s">
-        <v>11</v>
-      </c>
-      <c r="C8" t="s">
-        <v>7</v>
-      </c>
-      <c r="D8" t="n">
-        <v>0</v>
-      </c>
-      <c r="E8" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5">
-      <c r="A9" t="s">
-        <v>8</v>
-      </c>
-      <c r="B9" t="s">
-        <v>6</v>
-      </c>
-      <c r="C9" t="s">
-        <v>7</v>
-      </c>
-      <c r="D9" t="n">
-        <v>1.90094648465e-06</v>
-      </c>
-      <c r="E9" t="n">
         <v>1.9e-06</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Removed profiling from AllOuterReceptors module
</commit_message>
<xml_diff>
--- a/fixtures/output/01043110000366247_incidence.xlsx
+++ b/fixtures/output/01043110000366247_incidence.xlsx
@@ -430,7 +430,7 @@
         <v>7</v>
       </c>
       <c r="D2" t="n">
-        <v>1.80935904413e-06</v>
+        <v>1.80857518359e-06</v>
       </c>
       <c r="E2" t="n">
         <v>1.8e-06</v>
@@ -447,7 +447,7 @@
         <v>7</v>
       </c>
       <c r="D3" t="n">
-        <v>1.80935904413e-06</v>
+        <v>1.80857518359e-06</v>
       </c>
       <c r="E3" t="n">
         <v>1.8e-06</v>
@@ -464,7 +464,7 @@
         <v>7</v>
       </c>
       <c r="D4" t="n">
-        <v>1.80935904413e-06</v>
+        <v>1.80857518359e-06</v>
       </c>
       <c r="E4" t="n">
         <v>1.8e-06</v>
@@ -515,7 +515,7 @@
         <v>7</v>
       </c>
       <c r="D7" t="n">
-        <v>1.80935904413e-06</v>
+        <v>1.80857518359e-06</v>
       </c>
       <c r="E7" t="n">
         <v>1.8e-06</v>

</xml_diff>